<commit_message>
Wrote a new verion of kramer kappa (kramerKappa2.R) because the old ranking seemed to rank the selected categories last rather than first, and not assign the same rank to the remaining categories. The second version gives some odd results though and I'm not sure it's quite right. oro_type is ranked very low (k=0.3) when there should be high agreement
</commit_message>
<xml_diff>
--- a/outputs/coding/codingKappa.xlsx
+++ b/outputs/coding/codingKappa.xlsx
@@ -406,17 +406,9 @@
       <c r="C2">
         <v>0.9859376094797067</v>
       </c>
-      <c r="E2">
-        <v>0.08902255639097745</v>
-      </c>
       <c r="F2" t="inlineStr">
         <is>
           <t>Kendall's coeff of concordance</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>JP</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
discovered column naming error with m_co2_storage.Inorganic due to a mispelling of the word Multiple in the codebook. Have rectified the simplifyCodebookDistilbert.R function and re-written all the files
</commit_message>
<xml_diff>
--- a/outputs/coding/codingKappa.xlsx
+++ b/outputs/coding/codingKappa.xlsx
@@ -406,9 +406,17 @@
       <c r="C2">
         <v>0.9859376094797067</v>
       </c>
+      <c r="E2">
+        <v>0.08902255639097745</v>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
           <t>Kendall's coeff of concordance</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>JP</t>
         </is>
       </c>
     </row>
@@ -429,7 +437,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Kramer (1980)</t>
+          <t>kraemer (1980)</t>
         </is>
       </c>
     </row>
@@ -453,7 +461,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Kramer (1980)</t>
+          <t>kraemer (1980)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -479,7 +487,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Kramer (1980)</t>
+          <t>kraemer (1980)</t>
         </is>
       </c>
     </row>
@@ -500,7 +508,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Kramer (1980)</t>
+          <t>kraemer (1980)</t>
         </is>
       </c>
     </row>
@@ -511,17 +519,17 @@
         </is>
       </c>
       <c r="B7">
-        <v>0.5922677883625617</v>
+        <v>0.5837902834806478</v>
       </c>
       <c r="C7">
-        <v>0.9282502604838139</v>
+        <v>0.94862625852474</v>
       </c>
       <c r="D7">
-        <v>0.7972607103041887</v>
+        <v>0.7850223480679014</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Kramer (1980)</t>
+          <t>kraemer (1980)</t>
         </is>
       </c>
     </row>
@@ -545,7 +553,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Kramer (1980)</t>
+          <t>kraemer (1980)</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -574,7 +582,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Kramer (1980)</t>
+          <t>kraemer (1980)</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -603,7 +611,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Kramer (1980)</t>
+          <t>kraemer (1980)</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -632,7 +640,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Kramer (1980)</t>
+          <t>kraemer (1980)</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -658,7 +666,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Kramer (1980)</t>
+          <t>kraemer (1980)</t>
         </is>
       </c>
     </row>
@@ -682,7 +690,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Kramer (1980)</t>
+          <t>kraemer (1980)</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -711,7 +719,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Kramer (1980)</t>
+          <t>kraemer (1980)</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -756,17 +764,9 @@
       <c r="D16">
         <v>0.08432296231375996</v>
       </c>
-      <c r="E16">
-        <v>0.2603920051255966</v>
-      </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Kramer (1980)</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>JP</t>
+          <t>kraemer (1980)</t>
         </is>
       </c>
     </row>
@@ -790,7 +790,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Kramer (1980)</t>
+          <t>kraemer (1980)</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -845,7 +845,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Kramer (1980)</t>
+          <t>kraemer (1980)</t>
         </is>
       </c>
     </row>
@@ -866,7 +866,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Kramer (1980)</t>
+          <t>kraemer (1980)</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Kramer (1980)</t>
+          <t>kraemer (1980)</t>
         </is>
       </c>
     </row>
@@ -1180,7 +1180,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Kramer (1980)</t>
+          <t>kraemer (1980)</t>
         </is>
       </c>
     </row>
@@ -1201,7 +1201,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Kramer (1980)</t>
+          <t>kraemer (1980)</t>
         </is>
       </c>
     </row>
@@ -1222,7 +1222,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Kramer (1980)</t>
+          <t>kraemer (1980)</t>
         </is>
       </c>
     </row>

</xml_diff>